<commit_message>
Added DAC learning curve
</commit_message>
<xml_diff>
--- a/cost.xlsx
+++ b/cost.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/I577769/Documents/websites/carbon-removal-technologies-potential-cost/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thimo Merke\Google Drive\Dokumente\uni\23Spring\Bachelorarbeit\Plots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DBBC5A8-6C38-C349-B0B9-060FB03BACAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2811B834-29DD-4CD3-988E-92BA7AC48808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20780" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{4365A42F-3778-7F49-9C3F-9D1A66BDD8C8}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{4365A42F-3778-7F49-9C3F-9D1A66BDD8C8}"/>
   </bookViews>
   <sheets>
     <sheet name="cost" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">cost!$A$1:$C$35</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">cost!$A$1:$C$50</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="37">
   <si>
     <t>tech</t>
   </si>
@@ -62,68 +62,119 @@
     <t>Afforestation</t>
   </si>
   <si>
-    <t>Gorte</t>
-  </si>
-  <si>
     <t>NRC 2015</t>
   </si>
   <si>
-    <t>Fuss</t>
-  </si>
-  <si>
     <t>Enhanced Weathering</t>
   </si>
   <si>
-    <t>Beerling</t>
-  </si>
-  <si>
-    <t>Goll</t>
-  </si>
-  <si>
-    <t>Lackner</t>
-  </si>
-  <si>
-    <t>Knops</t>
-  </si>
-  <si>
     <t>Ocean Fertilization</t>
   </si>
   <si>
-    <t>Harrison</t>
-  </si>
-  <si>
-    <t>Jones</t>
-  </si>
-  <si>
-    <t>Gattuso</t>
-  </si>
-  <si>
     <t>Soil Sequestration</t>
   </si>
   <si>
-    <t>Bossio</t>
-  </si>
-  <si>
-    <t>Chambers</t>
-  </si>
-  <si>
     <t>NASEM 2018</t>
   </si>
   <si>
-    <t>Fuentes-George</t>
-  </si>
-  <si>
     <t>NASEM 2022</t>
+  </si>
+  <si>
+    <t>DAC</t>
+  </si>
+  <si>
+    <t>House 2011</t>
+  </si>
+  <si>
+    <t>Socolow 2011</t>
+  </si>
+  <si>
+    <t>Mazzotti 2013</t>
+  </si>
+  <si>
+    <t>Zeman 2014</t>
+  </si>
+  <si>
+    <t>Holmes and Keith 2012</t>
+  </si>
+  <si>
+    <t>Keith 2018</t>
+  </si>
+  <si>
+    <t>Kulkarni and Sholl 2012</t>
+  </si>
+  <si>
+    <t>Keith 2006</t>
+  </si>
+  <si>
+    <t>Climeworks</t>
+  </si>
+  <si>
+    <t>Nemet and Brandt 2012</t>
+  </si>
+  <si>
+    <t>NASEM 2019</t>
+  </si>
+  <si>
+    <t>NASEM 2020</t>
+  </si>
+  <si>
+    <t>NASEM 2021</t>
+  </si>
+  <si>
+    <t>Stolaroff 2008</t>
+  </si>
+  <si>
+    <t>Gorte 2009</t>
+  </si>
+  <si>
+    <t>Fuss 2018</t>
+  </si>
+  <si>
+    <t>Beerling 2018</t>
+  </si>
+  <si>
+    <t>Goll 2021</t>
+  </si>
+  <si>
+    <t>Lackner 1997</t>
+  </si>
+  <si>
+    <t>Knops 2021</t>
+  </si>
+  <si>
+    <t>Harrison 2013</t>
+  </si>
+  <si>
+    <t>Jones 2014</t>
+  </si>
+  <si>
+    <t>Gattuso 2021</t>
+  </si>
+  <si>
+    <t>Bossio 2020</t>
+  </si>
+  <si>
+    <t>Chambers 2016</t>
+  </si>
+  <si>
+    <t>Fuentes-George 2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -189,8 +240,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9FD96A0-84F3-5046-B58E-579B4267A792}" name="Table_cost" displayName="Table_cost" ref="A1:C35" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:C35" xr:uid="{D9FD96A0-84F3-5046-B58E-579B4267A792}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9FD96A0-84F3-5046-B58E-579B4267A792}" name="Table_cost" displayName="Table_cost" ref="A1:C50" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:C50" xr:uid="{D9FD96A0-84F3-5046-B58E-579B4267A792}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{373C9060-501C-8943-9598-B36D766BCF83}" uniqueName="1" name="tech" queryTableFieldId="1" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{F1F35093-7134-0E4E-B004-3E087EBED456}" uniqueName="2" name="price" queryTableFieldId="2"/>
@@ -497,18 +548,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52A9080D-411C-4343-8F82-CF55825FB29E}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,381 +572,547 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
         <v>49</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>494</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4">
         <v>129</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
         <v>7.5</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6">
         <v>22</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7">
         <v>55</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9">
         <v>18</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
       </c>
       <c r="B10">
         <v>50</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>7</v>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
       </c>
       <c r="B11">
         <v>480</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>7</v>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
       </c>
       <c r="B12">
         <v>100</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>7</v>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
       </c>
       <c r="B13">
         <v>500</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>7</v>
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
       </c>
       <c r="B14">
         <v>40</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>7</v>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
       </c>
       <c r="B15">
         <v>100</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>7</v>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
       </c>
       <c r="B16">
         <v>600</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>7</v>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
       </c>
       <c r="B17">
         <v>578</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>7</v>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
       </c>
       <c r="B18">
         <v>70</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>7</v>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
       </c>
       <c r="B19">
         <v>24</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>7</v>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
       </c>
       <c r="B20">
         <v>123</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>7</v>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
       </c>
       <c r="B21">
         <v>60</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
-        <v>7</v>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
       </c>
       <c r="B22">
         <v>200</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>457</v>
+      </c>
+      <c r="C24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <v>230</v>
+      </c>
+      <c r="C25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27">
+        <v>100</v>
+      </c>
+      <c r="C27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28">
+        <v>3.44</v>
+      </c>
+      <c r="C28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29">
+        <v>11.34</v>
+      </c>
+      <c r="C29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30">
+        <v>100</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>80</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34">
+        <v>6.76</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35">
+        <v>1000</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36">
+        <v>641</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B23">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37">
+        <v>528</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38">
+        <v>309</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39">
+        <v>336</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40">
+        <v>83</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41">
+        <v>82</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42">
+        <v>60</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43">
+        <v>165</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44">
+        <v>600</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45">
+        <v>200</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46">
+        <v>60</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25">
-        <v>457</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B26">
-        <v>230</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B27">
-        <v>10</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28">
-        <v>100</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B29">
-        <v>3.44</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30">
-        <v>11.34</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31">
-        <v>100</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32">
-        <v>2</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47">
+        <v>89</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="1" t="s">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48">
+        <v>877</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34">
-        <v>80</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35">
-        <v>6.76</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>21</v>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49">
+        <v>156</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50">
+        <v>506</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -909,7 +1128,7 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>